<commit_message>
mục kho số TMDT thêm cột cọc sim
</commit_message>
<xml_diff>
--- a/import-so-TMDT.xlsx
+++ b/import-so-TMDT.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
   <si>
     <t>STT</t>
   </si>
@@ -94,6 +94,12 @@
   </si>
   <si>
     <t>07888123460</t>
+  </si>
+  <si>
+    <t>Cọc sim</t>
+  </si>
+  <si>
+    <t>Cạnh</t>
   </si>
 </sst>
 </file>
@@ -413,10 +419,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -426,11 +432,12 @@
     <col min="4" max="4" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.7109375" customWidth="1"/>
+    <col min="10" max="10" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -450,22 +457,25 @@
         <v>5</v>
       </c>
       <c r="G1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -484,20 +494,23 @@
       <c r="F2" t="s">
         <v>14</v>
       </c>
-      <c r="G2">
+      <c r="G2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H2">
         <v>0</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>15</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>16</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -517,15 +530,18 @@
         <v>14</v>
       </c>
       <c r="G3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H3" t="s">
         <v>21</v>
       </c>
-      <c r="H3" s="2">
+      <c r="I3" s="2">
         <v>25324</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>16</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>22</v>
       </c>
     </row>

</xml_diff>

<commit_message>
mục kho số TMDT thêm cột Mã đơn hàng
</commit_message>
<xml_diff>
--- a/import-so-TMDT.xlsx
+++ b/import-so-TMDT.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="30">
   <si>
     <t>STT</t>
   </si>
@@ -100,6 +100,15 @@
   </si>
   <si>
     <t>Cạnh</t>
+  </si>
+  <si>
+    <t>Mã đơn hàng</t>
+  </si>
+  <si>
+    <t>DH1</t>
+  </si>
+  <si>
+    <t>DH2</t>
   </si>
 </sst>
 </file>
@@ -419,10 +428,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -435,9 +444,10 @@
     <col min="7" max="7" width="8.7109375" customWidth="1"/>
     <col min="10" max="10" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -472,10 +482,13 @@
         <v>9</v>
       </c>
       <c r="L1" t="s">
+        <v>27</v>
+      </c>
+      <c r="M1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -509,8 +522,11 @@
       <c r="K2" t="s">
         <v>17</v>
       </c>
+      <c r="L2" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -543,6 +559,9 @@
       </c>
       <c r="K3" t="s">
         <v>22</v>
+      </c>
+      <c r="L3" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>